<commit_message>
Added space on front of house for dining room and living room.
</commit_message>
<xml_diff>
--- a/Crested Hills/Floor Plans/Elevation Detail Points.xlsx
+++ b/Crested Hills/Floor Plans/Elevation Detail Points.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Terrain Points</t>
   </si>
@@ -195,6 +195,63 @@
   </si>
   <si>
     <t>offset</t>
+  </si>
+  <si>
+    <t>mb1</t>
+  </si>
+  <si>
+    <t>mb2</t>
+  </si>
+  <si>
+    <t>mb3</t>
+  </si>
+  <si>
+    <t>mb4</t>
+  </si>
+  <si>
+    <t>es1</t>
+  </si>
+  <si>
+    <t>es2</t>
+  </si>
+  <si>
+    <t>es3</t>
+  </si>
+  <si>
+    <t>es4</t>
+  </si>
+  <si>
+    <t>es5</t>
+  </si>
+  <si>
+    <t>w1</t>
+  </si>
+  <si>
+    <t>w2</t>
+  </si>
+  <si>
+    <t>w3</t>
+  </si>
+  <si>
+    <t>w4</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>ud1</t>
   </si>
 </sst>
 </file>
@@ -332,22 +389,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1112</c:v>
+                  <c:v>1412</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2761.6810220159796</c:v>
+                  <c:v>-2461.6810220159796</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3077.956477685656</c:v>
+                  <c:v>-2777.956477685656</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3210.7193332284769</c:v>
+                  <c:v>-2910.7193332284769</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3007.603007613262</c:v>
+                  <c:v>-2707.603007613262</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1323.6063094759675</c:v>
+                  <c:v>1623.6063094759675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,22 +416,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>718.99999999999989</c:v>
+                  <c:v>1119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>627.40635202571298</c:v>
+                  <c:v>1027.406352025713</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>511.94891406647417</c:v>
+                  <c:v>911.94891406647412</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.61672957521409</c:v>
+                  <c:v>528.61672957521409</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-200.97501163762121</c:v>
+                  <c:v>199.02498836237879</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2123.8170292682071</c:v>
+                  <c:v>-1723.8170292682071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -416,16 +473,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-645.24104579354093</c:v>
+                  <c:v>-345.24104579354093</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-242.85191668654738</c:v>
+                  <c:v>57.148083313452616</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>319.87816270568305</c:v>
+                  <c:v>619.87816270568305</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1258.8425175286372</c:v>
+                  <c:v>1558.8425175286372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,16 +494,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-1153.1899768186784</c:v>
+                  <c:v>-753.18997681867836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1045.4415265884202</c:v>
+                  <c:v>-645.44152658842017</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1072.3250394091426</c:v>
+                  <c:v>-672.32503940914262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1248.4007086537479</c:v>
+                  <c:v>-848.40070865374787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,19 +553,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1094.0823441425532</c:v>
+                  <c:v>1394.0823441425532</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1056.760304547151</c:v>
+                  <c:v>1356.760304547151</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>939.01086014027419</c:v>
+                  <c:v>1239.0108601402742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>812.30374651211912</c:v>
+                  <c:v>1112.3037465121192</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>685.4228824454209</c:v>
+                  <c:v>985.4228824454209</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,19 +577,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>582.73152517954327</c:v>
+                  <c:v>982.73152517954327</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144.8892949351864</c:v>
+                  <c:v>544.8892949351864</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-290.31143728252596</c:v>
+                  <c:v>109.68856271747404</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-676.20980471999064</c:v>
+                  <c:v>-276.20980471999064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1010.7918701469723</c:v>
+                  <c:v>-610.79187014697231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,16 +639,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-822.07198434548343</c:v>
+                  <c:v>-522.07198434548343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-867.50863661454184</c:v>
+                  <c:v>-567.50863661454184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-882.05039709840855</c:v>
+                  <c:v>-582.05039709840855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-868.23903074225746</c:v>
+                  <c:v>-568.23903074225746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -603,16 +660,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-1045.4718702112095</c:v>
+                  <c:v>-645.47187021120953</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-479.48059899744783</c:v>
+                  <c:v>-79.480598997447828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>126.85466117337278</c:v>
+                  <c:v>526.85466117337273</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>554.59820756550857</c:v>
+                  <c:v>954.59820756550857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,19 +719,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-1871.755206276225</c:v>
+                  <c:v>-1571.755206276225</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1609.5282768405971</c:v>
+                  <c:v>-1309.5282768405971</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1219.3916748681379</c:v>
+                  <c:v>-919.3916748681379</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-813.63031824373411</c:v>
+                  <c:v>-513.63031824373411</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-566.29487274793848</c:v>
+                  <c:v>-266.29487274793848</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -686,19 +743,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>176.94072149462818</c:v>
+                  <c:v>576.94072149462818</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-137.09600315223958</c:v>
+                  <c:v>262.90399684776042</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-255.14332551881364</c:v>
+                  <c:v>144.85667448118636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-327.69323760416478</c:v>
+                  <c:v>72.306762395835221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-376.84448617733426</c:v>
+                  <c:v>23.155513822665739</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1741,20 +1798,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46" customWidth="1"/>
-    <col min="5" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-    <col min="10" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="7" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
@@ -1854,10 +1913,10 @@
         <v>56</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
@@ -1984,11 +2043,11 @@
       </c>
       <c r="U6">
         <f>($R$1-R6+$R$2)*12+$U$2</f>
-        <v>1112</v>
+        <v>1412</v>
       </c>
       <c r="V6">
         <f>($S$1-S6+$S$2)*12+$V$2</f>
-        <v>718.99999999999989</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
@@ -2061,11 +2120,11 @@
       </c>
       <c r="U7">
         <f t="shared" ref="U7:U40" si="16">($R$1-R7+$R$2)*12+$U$2</f>
-        <v>-2761.6810220159796</v>
+        <v>-2461.6810220159796</v>
       </c>
       <c r="V7">
         <f t="shared" ref="V7:V40" si="17">($S$1-S7+$S$2)*12+$V$2</f>
-        <v>627.40635202571298</v>
+        <v>1027.406352025713</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
@@ -2138,11 +2197,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="16"/>
-        <v>-3077.956477685656</v>
+        <v>-2777.956477685656</v>
       </c>
       <c r="V8">
         <f t="shared" si="17"/>
-        <v>511.94891406647417</v>
+        <v>911.94891406647412</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
@@ -2215,11 +2274,11 @@
       </c>
       <c r="U9">
         <f t="shared" si="16"/>
-        <v>-3210.7193332284769</v>
+        <v>-2910.7193332284769</v>
       </c>
       <c r="V9">
         <f t="shared" si="17"/>
-        <v>128.61672957521409</v>
+        <v>528.61672957521409</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
@@ -2292,11 +2351,11 @@
       </c>
       <c r="U10">
         <f t="shared" si="16"/>
-        <v>-3007.603007613262</v>
+        <v>-2707.603007613262</v>
       </c>
       <c r="V10">
         <f t="shared" si="17"/>
-        <v>-200.97501163762121</v>
+        <v>199.02498836237879</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
@@ -2369,11 +2428,11 @@
       </c>
       <c r="U11">
         <f t="shared" si="16"/>
-        <v>1323.6063094759675</v>
+        <v>1623.6063094759675</v>
       </c>
       <c r="V11">
         <f t="shared" si="17"/>
-        <v>-2123.8170292682071</v>
+        <v>-1723.8170292682071</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
@@ -2451,11 +2510,14 @@
       </c>
       <c r="U14">
         <f t="shared" si="16"/>
-        <v>-645.24104579354093</v>
+        <v>-345.24104579354093</v>
       </c>
       <c r="V14">
         <f t="shared" si="17"/>
-        <v>-1153.1899768186784</v>
+        <v>-753.18997681867836</v>
+      </c>
+      <c r="W14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
@@ -2528,11 +2590,14 @@
       </c>
       <c r="U15">
         <f t="shared" si="16"/>
-        <v>-242.85191668654738</v>
+        <v>57.148083313452616</v>
       </c>
       <c r="V15">
         <f t="shared" si="17"/>
-        <v>-1045.4415265884202</v>
+        <v>-645.44152658842017</v>
+      </c>
+      <c r="W15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
@@ -2605,14 +2670,17 @@
       </c>
       <c r="U16">
         <f t="shared" si="16"/>
-        <v>319.87816270568305</v>
+        <v>619.87816270568305</v>
       </c>
       <c r="V16">
         <f t="shared" si="17"/>
-        <v>-1072.3250394091426</v>
+        <v>-672.32503940914262</v>
+      </c>
+      <c r="W16" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>13</v>
       </c>
@@ -2682,14 +2750,17 @@
       </c>
       <c r="U17">
         <f t="shared" si="16"/>
-        <v>1258.8425175286372</v>
+        <v>1558.8425175286372</v>
       </c>
       <c r="V17">
         <f t="shared" si="17"/>
-        <v>-1248.4007086537479</v>
+        <v>-848.40070865374787</v>
+      </c>
+      <c r="W17" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>14</v>
       </c>
@@ -2697,7 +2768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>15</v>
       </c>
@@ -2767,14 +2838,17 @@
       </c>
       <c r="U20">
         <f t="shared" si="16"/>
-        <v>1094.0823441425532</v>
+        <v>1394.0823441425532</v>
       </c>
       <c r="V20">
         <f t="shared" si="17"/>
-        <v>582.73152517954327</v>
+        <v>982.73152517954327</v>
+      </c>
+      <c r="W20" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>16</v>
       </c>
@@ -2844,14 +2918,17 @@
       </c>
       <c r="U21">
         <f t="shared" si="16"/>
-        <v>1056.760304547151</v>
+        <v>1356.760304547151</v>
       </c>
       <c r="V21">
         <f t="shared" si="17"/>
-        <v>144.8892949351864</v>
+        <v>544.8892949351864</v>
+      </c>
+      <c r="W21" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>17</v>
       </c>
@@ -2921,14 +2998,17 @@
       </c>
       <c r="U22">
         <f t="shared" si="16"/>
-        <v>939.01086014027419</v>
+        <v>1239.0108601402742</v>
       </c>
       <c r="V22">
         <f t="shared" si="17"/>
-        <v>-290.31143728252596</v>
+        <v>109.68856271747404</v>
+      </c>
+      <c r="W22" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>18</v>
       </c>
@@ -2998,14 +3078,17 @@
       </c>
       <c r="U23">
         <f t="shared" si="16"/>
-        <v>812.30374651211912</v>
+        <v>1112.3037465121192</v>
       </c>
       <c r="V23">
         <f t="shared" si="17"/>
-        <v>-676.20980471999064</v>
+        <v>-276.20980471999064</v>
+      </c>
+      <c r="W23" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>19</v>
       </c>
@@ -3075,19 +3158,22 @@
       </c>
       <c r="U24">
         <f t="shared" si="16"/>
-        <v>685.4228824454209</v>
+        <v>985.4228824454209</v>
       </c>
       <c r="V24">
         <f t="shared" si="17"/>
-        <v>-1010.7918701469723</v>
+        <v>-610.79187014697231</v>
+      </c>
+      <c r="W24" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>22</v>
       </c>
@@ -3157,14 +3243,17 @@
       </c>
       <c r="U27">
         <f t="shared" si="16"/>
-        <v>-822.07198434548343</v>
+        <v>-522.07198434548343</v>
       </c>
       <c r="V27">
         <f t="shared" si="17"/>
-        <v>-1045.4718702112095</v>
+        <v>-645.47187021120953</v>
+      </c>
+      <c r="W27" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>23</v>
       </c>
@@ -3234,14 +3323,17 @@
       </c>
       <c r="U28">
         <f t="shared" si="16"/>
-        <v>-867.50863661454184</v>
+        <v>-567.50863661454184</v>
       </c>
       <c r="V28">
         <f t="shared" si="17"/>
-        <v>-479.48059899744783</v>
+        <v>-79.480598997447828</v>
+      </c>
+      <c r="W28" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>24</v>
       </c>
@@ -3311,14 +3403,17 @@
       </c>
       <c r="U29">
         <f t="shared" si="16"/>
-        <v>-882.05039709840855</v>
+        <v>-582.05039709840855</v>
       </c>
       <c r="V29">
         <f t="shared" si="17"/>
-        <v>126.85466117337278</v>
+        <v>526.85466117337273</v>
+      </c>
+      <c r="W29" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>25</v>
       </c>
@@ -3388,19 +3483,22 @@
       </c>
       <c r="U30">
         <f t="shared" si="16"/>
-        <v>-868.23903074225746</v>
+        <v>-568.23903074225746</v>
       </c>
       <c r="V30">
         <f t="shared" si="17"/>
-        <v>554.59820756550857</v>
+        <v>954.59820756550857</v>
+      </c>
+      <c r="W30" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>27</v>
       </c>
@@ -3470,14 +3568,17 @@
       </c>
       <c r="U33">
         <f t="shared" si="16"/>
-        <v>-1871.755206276225</v>
+        <v>-1571.755206276225</v>
       </c>
       <c r="V33">
         <f t="shared" si="17"/>
-        <v>176.94072149462818</v>
+        <v>576.94072149462818</v>
+      </c>
+      <c r="W33" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>28</v>
       </c>
@@ -3547,14 +3648,17 @@
       </c>
       <c r="U34">
         <f t="shared" si="16"/>
-        <v>-1609.5282768405971</v>
+        <v>-1309.5282768405971</v>
       </c>
       <c r="V34">
         <f t="shared" si="17"/>
-        <v>-137.09600315223958</v>
+        <v>262.90399684776042</v>
+      </c>
+      <c r="W34" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>29</v>
       </c>
@@ -3624,14 +3728,17 @@
       </c>
       <c r="U35">
         <f t="shared" si="16"/>
-        <v>-1219.3916748681379</v>
+        <v>-919.3916748681379</v>
       </c>
       <c r="V35">
         <f t="shared" si="17"/>
-        <v>-255.14332551881364</v>
+        <v>144.85667448118636</v>
+      </c>
+      <c r="W35" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>30</v>
       </c>
@@ -3701,14 +3808,17 @@
       </c>
       <c r="U36">
         <f t="shared" si="16"/>
-        <v>-813.63031824373411</v>
+        <v>-513.63031824373411</v>
       </c>
       <c r="V36">
         <f t="shared" si="17"/>
-        <v>-327.69323760416478</v>
+        <v>72.306762395835221</v>
+      </c>
+      <c r="W36" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>31</v>
       </c>
@@ -3778,19 +3888,22 @@
       </c>
       <c r="U37">
         <f t="shared" si="16"/>
-        <v>-566.29487274793848</v>
+        <v>-266.29487274793848</v>
       </c>
       <c r="V37">
         <f t="shared" si="17"/>
-        <v>-376.84448617733426</v>
+        <v>23.155513822665739</v>
+      </c>
+      <c r="W37" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>33</v>
       </c>
@@ -3860,11 +3973,14 @@
       </c>
       <c r="U40">
         <f t="shared" si="16"/>
-        <v>-1050.3424120489829</v>
+        <v>-750.34241204898285</v>
       </c>
       <c r="V40">
         <f t="shared" si="17"/>
-        <v>125.43430697574207</v>
+        <v>525.43430697574206</v>
+      </c>
+      <c r="W40" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>